<commit_message>
added full checks now try to implement on serverless vercel
</commit_message>
<xml_diff>
--- a/formData.xlsx
+++ b/formData.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -520,9 +520,32 @@
         <v>11/18/2024, 10:40:29 PM</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Travel</v>
+      </c>
+      <c r="B6" t="str">
+        <v>1-2 Weeks</v>
+      </c>
+      <c r="C6" t="str">
+        <v>rktindia2003@gmail.com</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Ravikant Tiwari</v>
+      </c>
+      <c r="E6" t="str">
+        <v>8744883594</v>
+      </c>
+      <c r="F6" t="str">
+        <v>+40</v>
+      </c>
+      <c r="G6" t="str">
+        <v>11/18/2024, 11:26:48 PM</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>